<commit_message>
Actualice los datos de estra caarpeta
</commit_message>
<xml_diff>
--- a/Calculo_Pac.xlsx
+++ b/Calculo_Pac.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\Mi_destino_Pacha\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6C8227A8-7A05-4DEA-B782-F9FB3B9DC44E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC0E9C22-997C-4E15-8F2A-3B7A46E4B69E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="0" windowWidth="16590" windowHeight="10920" xr2:uid="{6000EAE8-C3BE-4617-8CCC-D0222CAC96D7}"/>
+    <workbookView xWindow="3810" yWindow="90" windowWidth="16590" windowHeight="10920" xr2:uid="{6000EAE8-C3BE-4617-8CCC-D0222CAC96D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,19 +25,22 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>teoria</t>
   </si>
   <si>
     <t>practica</t>
   </si>
+  <si>
+    <t>calculos de notas</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -45,16 +48,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -62,12 +85,83 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -382,51 +476,69 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C99567B-25F7-4860-820A-F57525505CFB}">
-  <dimension ref="A3:C6"/>
+  <dimension ref="A2:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B3" sqref="B3:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="5"/>
+    </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="2">
         <v>67</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="2">
         <f>(B3*7)/100</f>
         <v>4.6900000000000004</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="2">
         <v>100</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2">
         <f>(B4*3)/100</f>
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C5">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="2">
         <f>SUM(C3+C4)</f>
         <v>7.69</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C6">
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="7">
         <f>ROUND(C5,0)</f>
         <v>8</v>
       </c>
     </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:C2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>